<commit_message>
bổ sung giao diện
</commit_message>
<xml_diff>
--- a/_task.xlsx
+++ b/_task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cybersoft\15\Capstone\NextJS-Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BD2232-5B61-48B7-B5D0-361DAABADF46}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C5402C-98C2-45E0-A696-145F30D34618}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>AuthContext</t>
+  </si>
+  <si>
+    <t>BookingAdmin</t>
+  </si>
+  <si>
+    <t>LocationAdmin</t>
   </si>
 </sst>
 </file>
@@ -478,9 +484,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -495,12 +498,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -523,14 +520,23 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -762,10 +768,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K974"/>
+  <dimension ref="A1:K976"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -818,657 +824,713 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>45775</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>45775</v>
       </c>
-      <c r="E2" s="10">
-        <v>1</v>
-      </c>
-      <c r="F2" s="11" t="s">
+      <c r="E2" s="9">
+        <v>1</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="8">
         <v>45800</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="8">
         <v>45803</v>
       </c>
-      <c r="I2" s="10">
-        <v>1</v>
-      </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="12"/>
+      <c r="I2" s="9">
+        <v>1</v>
+      </c>
+      <c r="J2" s="10"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>45776</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>45776</v>
       </c>
-      <c r="E3" s="10">
-        <v>1</v>
-      </c>
-      <c r="F3" s="11" t="s">
+      <c r="E3" s="9">
+        <v>1</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="8">
         <v>45800</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="8">
         <v>45803</v>
       </c>
-      <c r="I3" s="10">
-        <v>1</v>
-      </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="12"/>
+      <c r="I3" s="9">
+        <v>1</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="11"/>
     </row>
     <row r="4" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>45778</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>45785</v>
       </c>
-      <c r="E4" s="10">
-        <v>1</v>
-      </c>
-      <c r="F4" s="11" t="s">
+      <c r="E4" s="9">
+        <v>1</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>45800</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <v>45803</v>
       </c>
-      <c r="I4" s="10">
-        <v>1</v>
-      </c>
-      <c r="J4" s="11"/>
-      <c r="K4" s="12"/>
+      <c r="I4" s="9">
+        <v>1</v>
+      </c>
+      <c r="J4" s="10"/>
+      <c r="K4" s="11"/>
     </row>
     <row r="5" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="23"/>
+      <c r="B5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>45778</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>45785</v>
       </c>
-      <c r="E5" s="10">
-        <v>1</v>
-      </c>
-      <c r="F5" s="11" t="s">
+      <c r="E5" s="9">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>45800</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <v>45803</v>
       </c>
-      <c r="I5" s="10">
-        <v>1</v>
-      </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="12"/>
+      <c r="I5" s="9">
+        <v>1</v>
+      </c>
+      <c r="J5" s="10"/>
+      <c r="K5" s="11"/>
     </row>
     <row r="6" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="23"/>
+      <c r="B6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>45778</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>45785</v>
       </c>
-      <c r="E6" s="10">
-        <v>1</v>
-      </c>
-      <c r="F6" s="11" t="s">
+      <c r="E6" s="9">
+        <v>1</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <v>45800</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="8">
         <v>45803</v>
       </c>
-      <c r="I6" s="10">
-        <v>1</v>
-      </c>
-      <c r="J6" s="11"/>
-      <c r="K6" s="12"/>
+      <c r="I6" s="9">
+        <v>1</v>
+      </c>
+      <c r="J6" s="10"/>
+      <c r="K6" s="11"/>
     </row>
     <row r="7" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="23"/>
+      <c r="B7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>45778</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>45785</v>
       </c>
-      <c r="E7" s="10">
-        <v>1</v>
-      </c>
-      <c r="F7" s="11" t="s">
+      <c r="E7" s="9">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <v>45800</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="8">
         <v>45803</v>
       </c>
-      <c r="I7" s="10">
-        <v>1</v>
-      </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="12"/>
+      <c r="I7" s="9">
+        <v>1</v>
+      </c>
+      <c r="J7" s="10"/>
+      <c r="K7" s="11"/>
     </row>
     <row r="8" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
-      <c r="B8" s="8" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>45778</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>45785</v>
       </c>
-      <c r="E8" s="10">
-        <v>1</v>
-      </c>
-      <c r="F8" s="11" t="s">
+      <c r="E8" s="9">
+        <v>1</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <v>45800</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="8">
         <v>45803</v>
       </c>
-      <c r="I8" s="10">
-        <v>1</v>
-      </c>
-      <c r="J8" s="11"/>
-      <c r="K8" s="12"/>
+      <c r="I8" s="9">
+        <v>1</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="11"/>
     </row>
     <row r="9" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>45779</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>45781</v>
       </c>
-      <c r="E9" s="10">
-        <v>1</v>
-      </c>
-      <c r="F9" s="11" t="s">
+      <c r="E9" s="9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <v>45800</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="8">
         <v>45803</v>
       </c>
-      <c r="I9" s="10">
-        <v>1</v>
-      </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="12"/>
+      <c r="I9" s="9">
+        <v>1</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="11"/>
     </row>
     <row r="10" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="8" t="s">
+      <c r="A10" s="23"/>
+      <c r="B10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>45779</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>45781</v>
       </c>
-      <c r="E10" s="10">
-        <v>1</v>
-      </c>
-      <c r="F10" s="11" t="s">
+      <c r="E10" s="9">
+        <v>1</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="8">
         <v>45800</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="8">
         <v>45803</v>
       </c>
-      <c r="I10" s="10">
-        <v>1</v>
-      </c>
-      <c r="J10" s="11"/>
-      <c r="K10" s="12"/>
+      <c r="I10" s="9">
+        <v>1</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="K10" s="11"/>
     </row>
     <row r="11" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="8" t="s">
+      <c r="A11" s="24"/>
+      <c r="B11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>45779</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>45781</v>
       </c>
-      <c r="E11" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="F11" s="11" t="s">
+      <c r="E11" s="9">
+        <v>1</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="8">
         <v>45800</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="8">
         <v>45803</v>
       </c>
-      <c r="I11" s="10">
-        <v>0.8</v>
-      </c>
-      <c r="J11" s="11"/>
-      <c r="K11" s="12"/>
+      <c r="I11" s="9">
+        <v>1</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="11"/>
     </row>
     <row r="12" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>45787</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <v>45792</v>
       </c>
-      <c r="E12" s="10">
-        <v>1</v>
-      </c>
-      <c r="F12" s="11" t="s">
+      <c r="E12" s="9">
+        <v>1</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="8">
         <v>45800</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="8">
         <v>45803</v>
       </c>
-      <c r="I12" s="10">
-        <v>0.8</v>
-      </c>
-      <c r="J12" s="11"/>
-      <c r="K12" s="12"/>
+      <c r="I12" s="9">
+        <v>1</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="11"/>
     </row>
     <row r="13" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="23"/>
+      <c r="B13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>45787</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <v>45792</v>
       </c>
-      <c r="E13" s="10">
-        <v>1</v>
-      </c>
-      <c r="F13" s="11" t="s">
+      <c r="E13" s="9">
+        <v>1</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <v>45800</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="8">
         <v>45803</v>
       </c>
-      <c r="I13" s="10">
-        <v>0.8</v>
-      </c>
-      <c r="J13" s="11"/>
-      <c r="K13" s="12"/>
+      <c r="I13" s="9">
+        <v>1</v>
+      </c>
+      <c r="J13" s="10"/>
+      <c r="K13" s="11"/>
     </row>
     <row r="14" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="8" t="s">
+      <c r="A14" s="23"/>
+      <c r="B14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>45787</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="8">
         <v>45792</v>
       </c>
-      <c r="E14" s="10">
-        <v>1</v>
-      </c>
-      <c r="F14" s="11" t="s">
+      <c r="E14" s="9">
+        <v>1</v>
+      </c>
+      <c r="F14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="8">
         <v>45800</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="8">
         <v>45803</v>
       </c>
-      <c r="I14" s="10">
-        <v>1</v>
-      </c>
-      <c r="J14" s="11"/>
-      <c r="K14" s="12"/>
+      <c r="I14" s="9">
+        <v>1</v>
+      </c>
+      <c r="J14" s="10"/>
+      <c r="K14" s="11"/>
     </row>
     <row r="15" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
-      <c r="B15" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="9">
-        <v>45787</v>
-      </c>
-      <c r="D15" s="9">
-        <v>45792</v>
-      </c>
-      <c r="E15" s="10">
-        <v>1</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="9">
-        <v>45800</v>
-      </c>
-      <c r="H15" s="9">
-        <v>45803</v>
-      </c>
-      <c r="I15" s="10">
-        <v>1</v>
-      </c>
-      <c r="J15" s="11"/>
-      <c r="K15" s="12"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="8">
+        <v>45802</v>
+      </c>
+      <c r="D15" s="8">
+        <v>45806</v>
+      </c>
+      <c r="E15" s="9">
+        <v>1</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="8">
+        <v>45807</v>
+      </c>
+      <c r="H15" s="8">
+        <v>45809</v>
+      </c>
+      <c r="I15" s="9">
+        <v>1</v>
+      </c>
+      <c r="J15" s="10"/>
+      <c r="K15" s="11"/>
     </row>
     <row r="16" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="23"/>
+      <c r="B16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="8">
+        <v>45802</v>
+      </c>
+      <c r="D16" s="8">
+        <v>45806</v>
+      </c>
+      <c r="E16" s="9">
+        <v>1</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="8">
+        <v>45807</v>
+      </c>
+      <c r="H16" s="8">
+        <v>45809</v>
+      </c>
+      <c r="I16" s="9">
+        <v>1</v>
+      </c>
+      <c r="J16" s="10"/>
+      <c r="K16" s="11"/>
+    </row>
+    <row r="17" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="24"/>
+      <c r="B17" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="8">
+        <v>45787</v>
+      </c>
+      <c r="D17" s="8">
+        <v>45792</v>
+      </c>
+      <c r="E17" s="9">
+        <v>1</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="8">
+        <v>45800</v>
+      </c>
+      <c r="H17" s="8">
+        <v>45803</v>
+      </c>
+      <c r="I17" s="9">
+        <v>1</v>
+      </c>
+      <c r="J17" s="10"/>
+      <c r="K17" s="11"/>
+    </row>
+    <row r="18" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A18" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C18" s="8">
         <v>45789</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D18" s="8">
         <v>45790</v>
       </c>
-      <c r="E16" s="10">
-        <v>1</v>
-      </c>
-      <c r="F16" s="11" t="s">
+      <c r="E18" s="9">
+        <v>1</v>
+      </c>
+      <c r="F18" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G18" s="8">
         <v>45800</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H18" s="8">
         <v>45803</v>
       </c>
-      <c r="I16" s="10">
-        <v>1</v>
-      </c>
-      <c r="J16" s="11"/>
-      <c r="K16" s="12"/>
-    </row>
-    <row r="17" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="9">
-        <v>45789</v>
-      </c>
-      <c r="D17" s="9">
-        <v>45790</v>
-      </c>
-      <c r="E17" s="10">
-        <v>1</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="9">
-        <v>45800</v>
-      </c>
-      <c r="H17" s="9">
-        <v>45803</v>
-      </c>
-      <c r="I17" s="10">
-        <v>1</v>
-      </c>
-      <c r="J17" s="11"/>
-      <c r="K17" s="12"/>
-    </row>
-    <row r="18" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="9">
-        <v>45789</v>
-      </c>
-      <c r="D18" s="9">
-        <v>45790</v>
-      </c>
-      <c r="E18" s="10">
-        <v>1</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="9">
-        <v>45800</v>
-      </c>
-      <c r="H18" s="9">
-        <v>45803</v>
-      </c>
-      <c r="I18" s="10">
-        <v>1</v>
-      </c>
-      <c r="J18" s="11"/>
-      <c r="K18" s="12"/>
+      <c r="I18" s="9">
+        <v>1</v>
+      </c>
+      <c r="J18" s="10"/>
+      <c r="K18" s="11"/>
     </row>
     <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
-      <c r="B19" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="9">
+      <c r="A19" s="23"/>
+      <c r="B19" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="8">
         <v>45789</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="8">
         <v>45790</v>
       </c>
-      <c r="E19" s="10">
-        <v>1</v>
-      </c>
-      <c r="F19" s="11" t="s">
+      <c r="E19" s="9">
+        <v>1</v>
+      </c>
+      <c r="F19" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="8">
         <v>45800</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="8">
         <v>45803</v>
       </c>
-      <c r="I19" s="10">
-        <v>1</v>
-      </c>
-      <c r="J19" s="11"/>
-      <c r="K19" s="12"/>
+      <c r="I19" s="9">
+        <v>1</v>
+      </c>
+      <c r="J19" s="10"/>
+      <c r="K19" s="11"/>
     </row>
     <row r="20" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="23"/>
+      <c r="B20" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="8">
+        <v>45789</v>
+      </c>
+      <c r="D20" s="8">
+        <v>45790</v>
+      </c>
+      <c r="E20" s="9">
+        <v>1</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="8">
+        <v>45800</v>
+      </c>
+      <c r="H20" s="8">
+        <v>45803</v>
+      </c>
+      <c r="I20" s="9">
+        <v>1</v>
+      </c>
+      <c r="J20" s="10"/>
+      <c r="K20" s="11"/>
+    </row>
+    <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="23"/>
+      <c r="B21" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="8">
+        <v>45789</v>
+      </c>
+      <c r="D21" s="8">
+        <v>45790</v>
+      </c>
+      <c r="E21" s="9">
+        <v>1</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="8">
+        <v>45800</v>
+      </c>
+      <c r="H21" s="8">
+        <v>45803</v>
+      </c>
+      <c r="I21" s="9">
+        <v>1</v>
+      </c>
+      <c r="J21" s="10"/>
+      <c r="K21" s="11"/>
+    </row>
+    <row r="22" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17">
+      <c r="B22" s="13"/>
+      <c r="C22" s="14">
         <v>45790</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D22" s="15">
         <v>45791</v>
       </c>
-      <c r="E20" s="19">
-        <v>1</v>
-      </c>
-      <c r="F20" s="20" t="s">
+      <c r="E22" s="16">
+        <v>1</v>
+      </c>
+      <c r="F22" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="18">
+      <c r="G22" s="15">
         <v>45800</v>
       </c>
-      <c r="H20" s="18">
+      <c r="H22" s="15">
         <v>45803</v>
       </c>
-      <c r="I20" s="19">
-        <v>1</v>
-      </c>
-      <c r="J20" s="20"/>
-      <c r="K20" s="21"/>
-    </row>
-    <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="17">
-        <v>45791</v>
-      </c>
-      <c r="D21" s="18">
-        <v>45792</v>
-      </c>
-      <c r="E21" s="19">
-        <v>1</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" s="18">
-        <v>45800</v>
-      </c>
-      <c r="H21" s="18">
-        <v>45803</v>
-      </c>
-      <c r="I21" s="19">
-        <v>1</v>
-      </c>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
-    </row>
-    <row r="22" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="17">
-        <v>45792</v>
-      </c>
-      <c r="D22" s="18">
-        <v>45793</v>
-      </c>
-      <c r="E22" s="19">
-        <v>1</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="18">
-        <v>45800</v>
-      </c>
-      <c r="H22" s="18">
-        <v>45803</v>
-      </c>
-      <c r="I22" s="19">
-        <v>1</v>
-      </c>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
+      <c r="I22" s="16">
+        <v>1</v>
+      </c>
+      <c r="J22" s="17"/>
+      <c r="K22" s="18"/>
     </row>
     <row r="23" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="23" t="s">
+      <c r="A23" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="14">
+        <v>45791</v>
+      </c>
+      <c r="D23" s="15">
+        <v>45792</v>
+      </c>
+      <c r="E23" s="16">
+        <v>1</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="15">
+        <v>45800</v>
+      </c>
+      <c r="H23" s="15">
+        <v>45803</v>
+      </c>
+      <c r="I23" s="16">
+        <v>1</v>
+      </c>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+    </row>
+    <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="21"/>
+      <c r="B24" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="14">
+        <v>45792</v>
+      </c>
+      <c r="D24" s="15">
+        <v>45793</v>
+      </c>
+      <c r="E24" s="16">
+        <v>1</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="15">
+        <v>45800</v>
+      </c>
+      <c r="H24" s="15">
+        <v>45803</v>
+      </c>
+      <c r="I24" s="16">
+        <v>1</v>
+      </c>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+    </row>
+    <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="21"/>
+      <c r="B25" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C25" s="14">
         <v>45793</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D25" s="15">
         <v>45794</v>
       </c>
-      <c r="E23" s="19">
-        <v>1</v>
-      </c>
-      <c r="F23" s="20" t="s">
+      <c r="E25" s="16">
+        <v>1</v>
+      </c>
+      <c r="F25" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G23" s="18">
+      <c r="G25" s="15">
         <v>45800</v>
       </c>
-      <c r="H23" s="18">
+      <c r="H25" s="15">
         <v>45803</v>
       </c>
-      <c r="I23" s="19">
-        <v>1</v>
-      </c>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
+      <c r="I25" s="16">
+        <v>1</v>
+      </c>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
     </row>
-    <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2418,16 +2480,18 @@
     <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A18:A21"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A8"/>
     <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A12:A17"/>
   </mergeCells>
-  <conditionalFormatting sqref="E2:E23 I2:I23">
+  <conditionalFormatting sqref="E2:E25 I2:I25">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>

</xml_diff>